<commit_message>
edit and end documentation
</commit_message>
<xml_diff>
--- a/SPORT REPORT.xlsx
+++ b/SPORT REPORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_PROJECTs\48_csvLogToExcel\csvLogToExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CD8C1B-1A0E-4F74-A92F-19B828DCCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EE638E-7E3B-4992-BE1A-F43D6EF12C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1374,7 +1374,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>